<commit_message>
Added dynamic weighting under the var name: dynamic_weighting_denominator
/
</commit_message>
<xml_diff>
--- a/upload_files/nihad-azimli-resume__text.xlsx
+++ b/upload_files/nihad-azimli-resume__text.xlsx
@@ -259,13 +259,13 @@
     <t>project : 1</t>
   </si>
   <si>
+    <t>python : 1</t>
+  </si>
+  <si>
     <t>analysis : 1</t>
   </si>
   <si>
     <t>databases : 2</t>
-  </si>
-  <si>
-    <t>python : 1</t>
   </si>
   <si>
     <t>27.77</t>
@@ -705,7 +705,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -713,7 +713,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -721,7 +721,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:11">

</xml_diff>